<commit_message>
2D Inertial Model Formulation
Adding new adaptive time-step.

Organized code.

Added functions for parts of Main While, reducing the coding.
</commit_message>
<xml_diff>
--- a/Input_Data_Sheets/General_Data_HydroPol2D.xlsx
+++ b/Input_Data_Sheets/General_Data_HydroPol2D.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d29a325a694f12f3/Documentos/GitHub/HydroPol2D/Input_Data_Sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{BC26BABE-0DD9-49F0-8698-434367B7D6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39AEC86B-04D2-4BDF-8A87-E82E887F4B85}"/>
+  <xr:revisionPtr revIDLastSave="52" documentId="13_ncr:1_{BC26BABE-0DD9-49F0-8698-434367B7D6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F47A23C5-0A0A-4995-AB1C-8F400BE52DA1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2516,7 +2516,7 @@
   <dimension ref="A1:AX2187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AQ12" sqref="AQ12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2709,7 +2709,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
@@ -2805,7 +2805,7 @@
         <v>34</v>
       </c>
       <c r="AQ3" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR3" s="12"/>
       <c r="AS3" s="12" t="s">
@@ -2951,7 +2951,7 @@
         <v>53</v>
       </c>
       <c r="E5" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -3033,7 +3033,7 @@
         <v>66</v>
       </c>
       <c r="AQ5" s="19">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="AR5" s="8" t="s">
         <v>67</v>
@@ -3559,7 +3559,7 @@
         <v>125</v>
       </c>
       <c r="E12" s="15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>

</xml_diff>